<commit_message>
actualizacion de indicadores de resultados primer trimestre 2025
</commit_message>
<xml_diff>
--- a/src/assets/content/estados-financieros/2025/primer-trimestre/03_INFORMACION_PROGRAMATICA/03_INDICADORES_DE_RESULTADOS.xlsx
+++ b/src/assets/content/estados-financieros/2025/primer-trimestre/03_INFORMACION_PROGRAMATICA/03_INDICADORES_DE_RESULTADOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utsalamancaedu-my.sharepoint.com/personal/zcampos_utsalamanca_edu_mx/Documents/1.- 2025/1er TRIMESTRE 2025/ESTADOS FINANCIEROS 2025 1ER TRIMESTRE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utsalamancaedu-my.sharepoint.com/personal/zcampos_utsalamanca_edu_mx/Documents/1.- 2025/SEVAC/SEVAC 2025-EVIDENCIA PREGUNTAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{801C7E98-7CCB-4C1E-98F6-378D9E5D1550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{792C3805-ABD1-4C18-BA67-A8AB91C1C63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="161">
   <si>
     <t>Instructivo</t>
   </si>
@@ -447,9 +447,6 @@
 B= Número de alumnos proyectados a atender.</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Alumnos</t>
   </si>
   <si>
@@ -578,6 +575,27 @@
   </si>
   <si>
     <t>P0811</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>El mes de cumplimiento es Diciembre</t>
+  </si>
+  <si>
+    <t>Indicador</t>
+  </si>
+  <si>
+    <t>El mes de cumplimiento es Junio, Octubre y Diciembre</t>
+  </si>
+  <si>
+    <t>El mes de Cumplimiento es febrero, Junio y octubre</t>
+  </si>
+  <si>
+    <t>El mes de Cumplimiento es mayo, septiembre y diciembre</t>
+  </si>
+  <si>
+    <t>El mes de Cumplimiento es Diciembre</t>
   </si>
 </sst>
 </file>
@@ -589,7 +607,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -667,6 +685,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -779,30 +803,26 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,8 +840,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -941,24 +962,29 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="18">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Millares 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Millares 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -976,6 +1002,7 @@
     <cellStyle name="Normal 6" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Normal 6 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Normal_141008Reportes Cuadros Institucionales-sectorialesADV" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Porcentaje" xfId="17" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1282,10 +1309,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y35"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1301,40 +1331,43 @@
     <col min="15" max="15" width="44" style="23" customWidth="1"/>
     <col min="16" max="16" width="14.140625" style="23" customWidth="1"/>
     <col min="17" max="18" width="42.7109375" style="23" customWidth="1"/>
-    <col min="19" max="22" width="12" style="23" customWidth="1"/>
-    <col min="23" max="23" width="13" style="23" customWidth="1"/>
-    <col min="24" max="24" width="14.42578125" style="22" customWidth="1"/>
+    <col min="19" max="23" width="12" style="23" customWidth="1"/>
+    <col min="24" max="24" width="13" style="23" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" style="22" customWidth="1"/>
+    <col min="26" max="26" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:27" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="40"/>
-    </row>
-    <row r="2" spans="1:25" ht="22.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+    </row>
+    <row r="2" spans="1:27" ht="22.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>85</v>
       </c>
@@ -1364,13 +1397,14 @@
       <c r="S2" s="17"/>
       <c r="T2" s="17"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="18" t="s">
+      <c r="V2" s="39"/>
+      <c r="W2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="W2" s="18"/>
       <c r="X2" s="18"/>
-    </row>
-    <row r="3" spans="1:25" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y2" s="18"/>
+    </row>
+    <row r="3" spans="1:27" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>50</v>
       </c>
@@ -1434,25 +1468,31 @@
       <c r="U3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="19" t="s">
+      <c r="V3" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="W3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="W3" s="20" t="s">
+      <c r="X3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="X3" s="20" t="s">
+      <c r="Y3" s="20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="Z3" s="38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>89</v>
@@ -1502,34 +1542,41 @@
       <c r="S4" s="37">
         <v>2100</v>
       </c>
-      <c r="T4" s="37" t="s">
+      <c r="T4" s="37">
+        <v>2100</v>
+      </c>
+      <c r="U4" s="37">
+        <v>0</v>
+      </c>
+      <c r="V4" s="41">
+        <f>+U4/T4</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="37">
+        <v>0</v>
+      </c>
+      <c r="X4" s="37">
+        <v>2100</v>
+      </c>
+      <c r="Y4" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="U4" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V4" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W4" s="37">
-        <v>2100</v>
-      </c>
-      <c r="X4" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y4" s="37" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="Z4" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA4" s="37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>92</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>89</v>
@@ -1565,7 +1612,7 @@
         <v>102</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P5" s="34" t="s">
         <v>100</v>
@@ -1574,39 +1621,46 @@
         <v>112</v>
       </c>
       <c r="R5" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S5" s="37">
         <v>3</v>
       </c>
-      <c r="T5" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="U5" s="37" t="s">
+      <c r="T5" s="37">
+        <v>3</v>
+      </c>
+      <c r="U5" s="37">
+        <v>0</v>
+      </c>
+      <c r="V5" s="41">
+        <f t="shared" ref="V5:V15" si="0">+U5/T5</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="37">
+        <v>0</v>
+      </c>
+      <c r="X5" s="37">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="V5" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W5" s="37">
-        <v>3</v>
-      </c>
-      <c r="X5" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y5" s="37" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="Z5" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA5" s="37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>93</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>94</v>
@@ -1642,7 +1696,7 @@
         <v>103</v>
       </c>
       <c r="O6" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P6" s="34" t="s">
         <v>100</v>
@@ -1651,39 +1705,46 @@
         <v>112</v>
       </c>
       <c r="R6" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S6" s="37">
         <v>1021</v>
       </c>
-      <c r="T6" s="37" t="s">
+      <c r="T6" s="37">
+        <v>1021</v>
+      </c>
+      <c r="U6" s="37">
+        <v>0</v>
+      </c>
+      <c r="V6" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X6" s="37">
+        <v>1021</v>
+      </c>
+      <c r="Y6" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="U6" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V6" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W6" s="37">
-        <v>1021</v>
-      </c>
-      <c r="X6" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y6" s="37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="Z6" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA6" s="37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="28" t="s">
         <v>93</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>94</v>
@@ -1719,7 +1780,7 @@
         <v>104</v>
       </c>
       <c r="O7" s="35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P7" s="34" t="s">
         <v>100</v>
@@ -1728,39 +1789,46 @@
         <v>112</v>
       </c>
       <c r="R7" s="36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S7" s="37">
         <v>2100</v>
       </c>
-      <c r="T7" s="37" t="s">
+      <c r="T7" s="37">
+        <v>2100</v>
+      </c>
+      <c r="U7" s="37">
+        <v>0</v>
+      </c>
+      <c r="V7" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X7" s="37">
+        <v>2100</v>
+      </c>
+      <c r="Y7" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="U7" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V7" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W7" s="37">
-        <v>2100</v>
-      </c>
-      <c r="X7" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y7" s="41" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="66" x14ac:dyDescent="0.2">
+      <c r="Z7" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA7" s="37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="66" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>93</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>94</v>
@@ -1796,7 +1864,7 @@
         <v>104</v>
       </c>
       <c r="O8" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P8" s="34" t="s">
         <v>100</v>
@@ -1805,39 +1873,46 @@
         <v>112</v>
       </c>
       <c r="R8" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S8" s="37">
         <v>56</v>
       </c>
-      <c r="T8" s="37" t="s">
+      <c r="T8" s="37">
+        <v>56</v>
+      </c>
+      <c r="U8" s="37">
+        <v>0</v>
+      </c>
+      <c r="V8" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X8" s="37">
+        <v>56</v>
+      </c>
+      <c r="Y8" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="U8" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V8" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W8" s="37">
-        <v>56</v>
-      </c>
-      <c r="X8" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y8" s="41" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="Z8" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA8" s="37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>93</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>94</v>
@@ -1873,7 +1948,7 @@
         <v>105</v>
       </c>
       <c r="O9" s="35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P9" s="34" t="s">
         <v>100</v>
@@ -1882,39 +1957,46 @@
         <v>112</v>
       </c>
       <c r="R9" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S9" s="37">
         <v>80</v>
       </c>
-      <c r="T9" s="37" t="s">
+      <c r="T9" s="37">
+        <v>80</v>
+      </c>
+      <c r="U9" s="37">
+        <v>0</v>
+      </c>
+      <c r="V9" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W9" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X9" s="37">
+        <v>80</v>
+      </c>
+      <c r="Y9" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="U9" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V9" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W9" s="37">
-        <v>80</v>
-      </c>
-      <c r="X9" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y9" s="37" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="Z9" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA9" s="37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>95</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>96</v>
@@ -1950,7 +2032,7 @@
         <v>106</v>
       </c>
       <c r="O10" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P10" s="34" t="s">
         <v>100</v>
@@ -1959,39 +2041,46 @@
         <v>112</v>
       </c>
       <c r="R10" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S10" s="37">
         <v>450</v>
       </c>
-      <c r="T10" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="U10" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V10" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W10" s="37">
+      <c r="T10" s="37">
         <v>450</v>
       </c>
-      <c r="X10" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y10" s="37" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="66" x14ac:dyDescent="0.2">
+      <c r="U10" s="37">
+        <v>163</v>
+      </c>
+      <c r="V10" s="41">
+        <f t="shared" si="0"/>
+        <v>0.36222222222222222</v>
+      </c>
+      <c r="W10" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X10" s="37">
+        <v>450</v>
+      </c>
+      <c r="Y10" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z10" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA10" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="66" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>95</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>96</v>
@@ -2027,7 +2116,7 @@
         <v>107</v>
       </c>
       <c r="O11" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P11" s="34" t="s">
         <v>100</v>
@@ -2036,39 +2125,46 @@
         <v>112</v>
       </c>
       <c r="R11" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S11" s="37">
         <v>1500</v>
       </c>
-      <c r="T11" s="37" t="s">
+      <c r="T11" s="37">
+        <v>1500</v>
+      </c>
+      <c r="U11" s="37">
+        <v>0</v>
+      </c>
+      <c r="V11" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X11" s="37">
+        <v>1500</v>
+      </c>
+      <c r="Y11" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="U11" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V11" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W11" s="37">
-        <v>1500</v>
-      </c>
-      <c r="X11" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y11" s="37" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="Z11" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA11" s="37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>97</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>98</v>
@@ -2104,7 +2200,7 @@
         <v>108</v>
       </c>
       <c r="O12" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P12" s="34" t="s">
         <v>100</v>
@@ -2113,39 +2209,46 @@
         <v>112</v>
       </c>
       <c r="R12" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S12" s="37">
         <v>1</v>
       </c>
-      <c r="T12" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="U12" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V12" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W12" s="37">
+      <c r="T12" s="37">
         <v>1</v>
       </c>
-      <c r="X12" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y12" s="37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="U12" s="37">
+        <v>0</v>
+      </c>
+      <c r="V12" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W12" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X12" s="37">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z12" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA12" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>97</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>98</v>
@@ -2181,7 +2284,7 @@
         <v>108</v>
       </c>
       <c r="O13" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="34" t="s">
         <v>100</v>
@@ -2190,39 +2293,46 @@
         <v>112</v>
       </c>
       <c r="R13" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S13" s="37">
         <v>1</v>
       </c>
-      <c r="T13" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="U13" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V13" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W13" s="37">
+      <c r="T13" s="37">
         <v>1</v>
       </c>
-      <c r="X13" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y13" s="37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="U13" s="37">
+        <v>0</v>
+      </c>
+      <c r="V13" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X13" s="37">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z13" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA13" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>97</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>98</v>
@@ -2258,7 +2368,7 @@
         <v>109</v>
       </c>
       <c r="O14" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P14" s="34" t="s">
         <v>100</v>
@@ -2267,39 +2377,46 @@
         <v>112</v>
       </c>
       <c r="R14" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="S14" s="37">
         <v>95</v>
       </c>
-      <c r="T14" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="U14" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V14" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W14" s="37">
+      <c r="T14" s="37">
         <v>95</v>
       </c>
-      <c r="X14" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="Y14" s="37" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="U14" s="37">
+        <v>0</v>
+      </c>
+      <c r="V14" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X14" s="37">
+        <v>95</v>
+      </c>
+      <c r="Y14" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z14" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA14" s="37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>98</v>
@@ -2335,7 +2452,7 @@
         <v>110</v>
       </c>
       <c r="O15" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="34" t="s">
         <v>100</v>
@@ -2344,31 +2461,38 @@
         <v>112</v>
       </c>
       <c r="R15" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S15" s="37">
         <v>1680</v>
       </c>
-      <c r="T15" s="37" t="s">
-        <v>114</v>
+      <c r="T15" s="37">
+        <v>1680</v>
       </c>
       <c r="U15" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="V15" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="W15" s="37">
+        <v>117</v>
+      </c>
+      <c r="V15" s="41" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W15" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="X15" s="37">
         <v>1680</v>
       </c>
-      <c r="X15" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y15" s="37" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="Y15" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z15" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA15" s="37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
@@ -2502,10 +2626,10 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="A1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="24" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2962,12 +3086,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3085,15 +3206,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F51EF88-68BC-4A76-B5D9-47B8734FF48E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDF2C03A-FAFE-4FBB-9F24-298C907734CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3115,16 +3246,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDF2C03A-FAFE-4FBB-9F24-298C907734CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F51EF88-68BC-4A76-B5D9-47B8734FF48E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>